<commit_message>
Julia init & py-julia framework test
</commit_message>
<xml_diff>
--- a/Case_33BW_Data.xlsx
+++ b/Case_33BW_Data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Academic\SelfHealing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\IL_Self_Healing\IL_Self_Healing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EEBAF2-FB9F-4CF3-A851-8BD2D5F59833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1849FC26-2FC2-4B2E-B923-CE0B29528B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bus_Data" sheetId="9" r:id="rId1"/>
-    <sheet name="DG_Data" sheetId="16" r:id="rId2"/>
-    <sheet name="Branch_Data" sheetId="13" r:id="rId3"/>
-    <sheet name="Plot_Data" sheetId="14" r:id="rId4"/>
+    <sheet name="Bus" sheetId="9" r:id="rId1"/>
+    <sheet name="DG" sheetId="16" r:id="rId2"/>
+    <sheet name="Branch" sheetId="13" r:id="rId3"/>
+    <sheet name="Plot" sheetId="14" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>To</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,10 @@
   </si>
   <si>
     <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TieLine</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -187,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -210,11 +214,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,6 +245,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,19 +533,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BC601C-6925-4DEF-89B0-5C277128F18A}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -535,75 +556,75 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>0.1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>0.06</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <v>0.09</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
         <v>0.12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>0.06</v>
       </c>
       <c r="C6" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C7" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>0.2</v>
@@ -612,20 +633,20 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>0.06</v>
@@ -634,31 +655,31 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>12</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>0.06</v>
@@ -667,42 +688,42 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
         <v>0.12</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>15</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>0.06</v>
       </c>
       <c r="C16" s="2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>0.06</v>
@@ -711,20 +732,20 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>19</v>
       </c>
       <c r="B19" s="2">
         <v>0.09</v>
@@ -733,9 +754,9 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>0.09</v>
@@ -744,9 +765,9 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>0.09</v>
@@ -755,9 +776,9 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>0.09</v>
@@ -766,31 +787,31 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>0.09</v>
       </c>
       <c r="C23" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="C24" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>24</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>25</v>
       </c>
       <c r="B25" s="2">
         <v>0.42</v>
@@ -799,20 +820,20 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>26</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="C26" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>27</v>
       </c>
       <c r="B27" s="2">
         <v>0.06</v>
@@ -821,69 +842,80 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>0.06</v>
       </c>
       <c r="C28" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C29" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="2">
         <v>0.12</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C30" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="2">
         <v>0.2</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="2">
         <v>0.15</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="2">
         <v>0.21</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C33" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="2">
         <v>0.06</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>0.04</v>
       </c>
     </row>
@@ -898,20 +930,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC95A016-9E3A-444D-BA06-B44D9BEF325F}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -934,7 +966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -957,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -980,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1003,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1026,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1049,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1072,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1103,18 +1135,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24793DA6-4E57-4A6F-B748-31D49F9D3CC2}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -1133,8 +1165,11 @@
       <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1153,8 +1188,11 @@
       <c r="F2" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1173,8 +1211,11 @@
       <c r="F3" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1193,8 +1234,11 @@
       <c r="F4" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1213,8 +1257,11 @@
       <c r="F5" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1233,8 +1280,11 @@
       <c r="F6" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1253,8 +1303,11 @@
       <c r="F7" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1273,8 +1326,11 @@
       <c r="F8" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1293,8 +1349,11 @@
       <c r="F9" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1313,8 +1372,11 @@
       <c r="F10" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1333,8 +1395,11 @@
       <c r="F11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1353,8 +1418,11 @@
       <c r="F12" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1373,8 +1441,11 @@
       <c r="F13" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1393,8 +1464,11 @@
       <c r="F14" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1413,8 +1487,11 @@
       <c r="F15" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1433,8 +1510,11 @@
       <c r="F16" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1453,8 +1533,11 @@
       <c r="F17" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1473,8 +1556,11 @@
       <c r="F18" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1493,8 +1579,11 @@
       <c r="F19" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1513,8 +1602,11 @@
       <c r="F20" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1533,8 +1625,11 @@
       <c r="F21" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1553,8 +1648,11 @@
       <c r="F22" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1573,8 +1671,11 @@
       <c r="F23" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1593,8 +1694,11 @@
       <c r="F24" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1613,8 +1717,11 @@
       <c r="F25" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1633,8 +1740,11 @@
       <c r="F26" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1653,8 +1763,11 @@
       <c r="F27" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1673,8 +1786,11 @@
       <c r="F28" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1693,8 +1809,11 @@
       <c r="F29" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1713,8 +1832,11 @@
       <c r="F30" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1733,8 +1855,11 @@
       <c r="F31" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1753,8 +1878,11 @@
       <c r="F32" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1773,8 +1901,11 @@
       <c r="F33" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1793,8 +1924,11 @@
       <c r="F34" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1813,8 +1947,11 @@
       <c r="F35" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1833,8 +1970,11 @@
       <c r="F36" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1853,8 +1993,11 @@
       <c r="F37" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -1872,6 +2015,9 @@
       </c>
       <c r="F38" s="3">
         <v>10</v>
+      </c>
+      <c r="G38" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1888,9 +2034,9 @@
       <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="6" t="s">
         <v>9</v>
@@ -1899,7 +2045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1910,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1921,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1932,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1943,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1954,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1965,7 +2111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1976,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1987,7 +2133,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1998,7 +2144,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2009,7 +2155,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2020,7 +2166,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2031,7 +2177,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2042,7 +2188,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2053,7 +2199,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2064,7 +2210,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2075,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2086,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2097,7 +2243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2108,7 +2254,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2119,7 +2265,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2130,7 +2276,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2141,7 +2287,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2152,7 +2298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2163,7 +2309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2174,7 +2320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2185,7 +2331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2196,7 +2342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2207,7 +2353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2218,7 +2364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2229,7 +2375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2240,7 +2386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2251,7 +2397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>

</xml_diff>